<commit_message>
Added PTFE Tube Guide
## 2022-02-19

- Focusing on wiring today.
- `Connectors.xlsx` has a new tab for "Upper Level Wiring". This is wiring from the lower level patch panel up, e.g. to the hotend fans. Every connector has a pin count, recommended wire gauge, and approximate length needed. More will be filled in during disassembly.
- Added PN100, a PTFE tube guide to keep it from snagging the belts. The tube will now exit out of the back right, passing near the rear belts on the way. This will keep it out of the way and anchor it while the hotend moves.
- Top panel and hatch are modeled with a piano hinge.

## 2022-02-18

- Added twin cutouts to the side panels. Right side cutout is for PTFE conduit, the left side is for exhaust.
- Still considering approachs to wiring for the hotend.
</commit_message>
<xml_diff>
--- a/BOM/Printed Part List.xlsx
+++ b/BOM/Printed Part List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50B9A5E9-D578-467F-B4E3-793AADF262B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7E7E51-9349-4591-92E5-5DF8DB0BAF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="-27945" yWindow="2715" windowWidth="23250" windowHeight="12480" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="000 - Printed Parts" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="702" uniqueCount="323">
   <si>
     <t>Component</t>
   </si>
@@ -994,6 +994,15 @@
   </si>
   <si>
     <t>99 - XY - Motion - Y Axis Front Rail Guide.stl</t>
+  </si>
+  <si>
+    <t>PN100</t>
+  </si>
+  <si>
+    <t>Rear PTFE Tube Guide</t>
+  </si>
+  <si>
+    <t>100 - XY - Wiring - Rear PTFE Tube Guide.stl</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1069,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I95" totalsRowShown="0">
-  <autoFilter ref="A1:I95" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I84">
-    <sortCondition ref="A1:A84"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I96" totalsRowShown="0">
+  <autoFilter ref="A1:I96" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I85">
+    <sortCondition ref="A1:A85"/>
   </sortState>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{A8EA61BD-839A-4759-B873-CEDA7BEA684B}" name="Number"/>
@@ -1377,10 +1386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M81" sqref="M81"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I75" sqref="I75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3394,33 +3403,33 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>256</v>
+        <v>320</v>
       </c>
       <c r="B75" t="s">
-        <v>127</v>
+        <v>4</v>
       </c>
       <c r="C75" t="s">
-        <v>128</v>
+        <v>99</v>
       </c>
       <c r="D75" t="s">
         <v>1</v>
       </c>
       <c r="E75" t="s">
-        <v>257</v>
+        <v>321</v>
       </c>
       <c r="F75" t="s">
         <v>53</v>
       </c>
       <c r="G75">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>259</v>
+        <v>322</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B76" t="s">
         <v>127</v>
@@ -3432,7 +3441,7 @@
         <v>1</v>
       </c>
       <c r="E76" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F76" t="s">
         <v>53</v>
@@ -3441,12 +3450,12 @@
         <v>3</v>
       </c>
       <c r="I76" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
       <c r="B77" t="s">
         <v>127</v>
@@ -3455,27 +3464,24 @@
         <v>128</v>
       </c>
       <c r="D77" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
-        <v>129</v>
+        <v>258</v>
       </c>
       <c r="F77" t="s">
         <v>53</v>
       </c>
       <c r="G77">
-        <v>1</v>
-      </c>
-      <c r="H77" t="s">
-        <v>270</v>
+        <v>3</v>
       </c>
       <c r="I77" t="s">
-        <v>130</v>
+        <v>260</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B78" t="s">
         <v>127</v>
@@ -3484,10 +3490,10 @@
         <v>128</v>
       </c>
       <c r="D78" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E78" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="F78" t="s">
         <v>53</v>
@@ -3496,15 +3502,15 @@
         <v>1</v>
       </c>
       <c r="H78" t="s">
-        <v>139</v>
+        <v>270</v>
       </c>
       <c r="I78" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B79" t="s">
         <v>127</v>
@@ -3513,10 +3519,10 @@
         <v>128</v>
       </c>
       <c r="D79" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E79" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F79" t="s">
         <v>53</v>
@@ -3525,15 +3531,15 @@
         <v>1</v>
       </c>
       <c r="H79" t="s">
-        <v>271</v>
+        <v>139</v>
       </c>
       <c r="I79" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>174</v>
+        <v>236</v>
       </c>
       <c r="B80" t="s">
         <v>127</v>
@@ -3542,10 +3548,10 @@
         <v>128</v>
       </c>
       <c r="D80" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E80" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F80" t="s">
         <v>53</v>
@@ -3554,15 +3560,15 @@
         <v>1</v>
       </c>
       <c r="H80" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I80" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>235</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
         <v>127</v>
@@ -3571,24 +3577,27 @@
         <v>128</v>
       </c>
       <c r="D81" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E81" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="F81" t="s">
         <v>53</v>
       </c>
       <c r="G81">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="H81" t="s">
+        <v>272</v>
       </c>
       <c r="I81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="B82" t="s">
         <v>127</v>
@@ -3600,21 +3609,21 @@
         <v>1</v>
       </c>
       <c r="E82" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="F82" t="s">
         <v>53</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I82" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B83" t="s">
         <v>127</v>
@@ -3626,7 +3635,7 @@
         <v>1</v>
       </c>
       <c r="E83" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="F83" t="s">
         <v>53</v>
@@ -3635,12 +3644,12 @@
         <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B84" t="s">
         <v>127</v>
@@ -3652,7 +3661,7 @@
         <v>1</v>
       </c>
       <c r="E84" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F84" t="s">
         <v>53</v>
@@ -3661,38 +3670,38 @@
         <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>275</v>
+        <v>227</v>
       </c>
       <c r="B85" t="s">
-        <v>278</v>
+        <v>127</v>
       </c>
       <c r="C85" t="s">
-        <v>281</v>
+        <v>128</v>
       </c>
       <c r="D85" t="s">
         <v>1</v>
       </c>
       <c r="E85" t="s">
-        <v>279</v>
+        <v>158</v>
       </c>
       <c r="F85" t="s">
-        <v>293</v>
+        <v>53</v>
       </c>
       <c r="G85">
         <v>1</v>
       </c>
       <c r="I85" t="s">
-        <v>282</v>
+        <v>159</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B86" t="s">
         <v>278</v>
@@ -3704,21 +3713,21 @@
         <v>1</v>
       </c>
       <c r="E86" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F86" t="s">
         <v>293</v>
       </c>
       <c r="G86">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I86" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B87" t="s">
         <v>278</v>
@@ -3730,33 +3739,33 @@
         <v>1</v>
       </c>
       <c r="E87" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="F87" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I87" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="B88" t="s">
         <v>278</v>
       </c>
       <c r="C88" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D88" t="s">
         <v>1</v>
       </c>
       <c r="E88" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="F88" t="s">
         <v>292</v>
@@ -3765,12 +3774,12 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="B89" t="s">
         <v>278</v>
@@ -3782,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="F89" t="s">
         <v>292</v>
@@ -3791,15 +3800,15 @@
         <v>1</v>
       </c>
       <c r="I89" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="B90" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C90" t="s">
         <v>287</v>
@@ -3808,85 +3817,85 @@
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F90" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I90" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B91" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="C91" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D91" t="s">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="F91" t="s">
         <v>293</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I91" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B92" t="s">
         <v>278</v>
       </c>
       <c r="C92" t="s">
-        <v>36</v>
+        <v>300</v>
       </c>
       <c r="D92" t="s">
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="F92" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G92">
         <v>1</v>
       </c>
       <c r="I92" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>299</v>
+        <v>312</v>
       </c>
       <c r="B93" t="s">
         <v>278</v>
       </c>
       <c r="C93" t="s">
-        <v>300</v>
+        <v>36</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="F93" t="s">
         <v>292</v>
@@ -3895,12 +3904,12 @@
         <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B94" t="s">
         <v>278</v>
@@ -3912,24 +3921,24 @@
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="F94" t="s">
         <v>292</v>
       </c>
       <c r="G94">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I94" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B95" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C95" t="s">
         <v>300</v>
@@ -3938,15 +3947,41 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="F95" t="s">
         <v>292</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I95" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>302</v>
+      </c>
+      <c r="B96" t="s">
+        <v>295</v>
+      </c>
+      <c r="C96" t="s">
+        <v>300</v>
+      </c>
+      <c r="D96" t="s">
+        <v>1</v>
+      </c>
+      <c r="E96" t="s">
+        <v>305</v>
+      </c>
+      <c r="F96" t="s">
+        <v>292</v>
+      </c>
+      <c r="G96">
+        <v>1</v>
+      </c>
+      <c r="I96" t="s">
         <v>307</v>
       </c>
     </row>

</xml_diff>

<commit_message>
New couplers, lots of part list fixes
## 2022-02-25

- Lots of part corrections in the model.
- Modeled and added the 3mm spring steel build plate.
- Finished the front door and related components in the model. Added M5x14 FHCS to the BOM.
- Cleaned up the frame components to be external references instead of internal. Will fix the XY and rest of Z axis tomorrow.
- PTFE coupler and hose exhaust work well--will need TPU guide between the pneumatic couplers to align the PTFE tubes.

## 2022-02-24

- Assembled and measured door. Approximate clearance with MISUMI hinges is 4-5mm on the handle side.
- FPD of hose exhaust and PTFE coupler for side panels. Adding PN120 and PN121.
- Testing stability of door. I've mocked up spacers that are as thick as the paneling, but I believe they are allowing the door to sag.
- Modified PN092, the frame base foot, to work with BHCS.
- Corrected a few file names against the master log.
</commit_message>
<xml_diff>
--- a/BOM/Printed Part List.xlsx
+++ b/BOM/Printed Part List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551003AF-69E0-48E1-8BEC-8AAE4F0E4910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A524F4CD-6EC6-4A76-A7B7-E62FBD692993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27600" yWindow="3060" windowWidth="23250" windowHeight="12480" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
+    <workbookView xWindow="-27255" yWindow="3405" windowWidth="23250" windowHeight="12480" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
   <sheets>
     <sheet name="000 - Printed Parts" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="332">
   <si>
     <t>Component</t>
   </si>
@@ -1012,6 +1012,24 @@
   </si>
   <si>
     <t>89 - XY - Motion - Stepper Alignment Slider.stl</t>
+  </si>
+  <si>
+    <t>PN120</t>
+  </si>
+  <si>
+    <t>Exterior PTFE Coupler</t>
+  </si>
+  <si>
+    <t>120 - Exterior - Frame - Exterior PTFE Coupler.stl</t>
+  </si>
+  <si>
+    <t>PN121</t>
+  </si>
+  <si>
+    <t>Exhaust Hose Coupler</t>
+  </si>
+  <si>
+    <t>121 - Exterior - Frame - Exhaust Hose Coupler.stl</t>
   </si>
 </sst>
 </file>
@@ -1078,8 +1096,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I97" totalsRowShown="0">
-  <autoFilter ref="A1:I97" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5F341AE2-224B-4051-B04D-BA10CC5651EC}" name="Table1" displayName="Table1" ref="A1:I99" totalsRowShown="0">
+  <autoFilter ref="A1:I99" xr:uid="{7A633D33-D295-46C3-AB03-03E2AB6E078E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:I86">
     <sortCondition ref="A1:A86"/>
   </sortState>
@@ -1395,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
-  <dimension ref="A1:I97"/>
+  <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I65" sqref="I65"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3736,59 +3754,59 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>275</v>
+        <v>326</v>
       </c>
       <c r="B87" t="s">
-        <v>278</v>
+        <v>127</v>
       </c>
       <c r="C87" t="s">
-        <v>281</v>
+        <v>38</v>
       </c>
       <c r="D87" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E87" t="s">
-        <v>279</v>
+        <v>327</v>
       </c>
       <c r="F87" t="s">
-        <v>293</v>
+        <v>53</v>
       </c>
       <c r="G87">
         <v>1</v>
       </c>
       <c r="I87" t="s">
-        <v>282</v>
+        <v>328</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>276</v>
+        <v>329</v>
       </c>
       <c r="B88" t="s">
-        <v>278</v>
+        <v>127</v>
       </c>
       <c r="C88" t="s">
-        <v>281</v>
+        <v>38</v>
       </c>
       <c r="D88" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E88" t="s">
-        <v>280</v>
+        <v>330</v>
       </c>
       <c r="F88" t="s">
-        <v>293</v>
+        <v>53</v>
       </c>
       <c r="G88">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>283</v>
+        <v>331</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B89" t="s">
         <v>278</v>
@@ -3800,59 +3818,59 @@
         <v>1</v>
       </c>
       <c r="E89" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="F89" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G89">
         <v>1</v>
       </c>
       <c r="I89" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B90" t="s">
         <v>278</v>
       </c>
       <c r="C90" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D90" t="s">
         <v>1</v>
       </c>
       <c r="E90" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="F90" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I90" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B91" t="s">
         <v>278</v>
       </c>
       <c r="C91" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="D91" t="s">
         <v>1</v>
       </c>
       <c r="E91" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F91" t="s">
         <v>292</v>
@@ -3861,15 +3879,15 @@
         <v>1</v>
       </c>
       <c r="I91" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B92" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C92" t="s">
         <v>287</v>
@@ -3878,73 +3896,73 @@
         <v>1</v>
       </c>
       <c r="E92" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="F92" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G92">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I92" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>309</v>
+        <v>290</v>
       </c>
       <c r="B93" t="s">
         <v>278</v>
       </c>
       <c r="C93" t="s">
-        <v>300</v>
+        <v>287</v>
       </c>
       <c r="D93" t="s">
         <v>1</v>
       </c>
       <c r="E93" t="s">
-        <v>310</v>
+        <v>291</v>
       </c>
       <c r="F93" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G93">
         <v>1</v>
       </c>
       <c r="I93" t="s">
-        <v>311</v>
+        <v>294</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="B94" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
       <c r="C94" t="s">
-        <v>36</v>
+        <v>287</v>
       </c>
       <c r="D94" t="s">
         <v>1</v>
       </c>
       <c r="E94" t="s">
-        <v>313</v>
+        <v>296</v>
       </c>
       <c r="F94" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I94" t="s">
-        <v>314</v>
+        <v>297</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>299</v>
+        <v>309</v>
       </c>
       <c r="B95" t="s">
         <v>278</v>
@@ -3956,50 +3974,50 @@
         <v>1</v>
       </c>
       <c r="E95" t="s">
-        <v>304</v>
+        <v>310</v>
       </c>
       <c r="F95" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G95">
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>306</v>
+        <v>311</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>301</v>
+        <v>312</v>
       </c>
       <c r="B96" t="s">
         <v>278</v>
       </c>
       <c r="C96" t="s">
-        <v>300</v>
+        <v>36</v>
       </c>
       <c r="D96" t="s">
         <v>1</v>
       </c>
       <c r="E96" t="s">
-        <v>303</v>
+        <v>313</v>
       </c>
       <c r="F96" t="s">
         <v>292</v>
       </c>
       <c r="G96">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I96" t="s">
-        <v>308</v>
+        <v>314</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="B97" t="s">
-        <v>295</v>
+        <v>278</v>
       </c>
       <c r="C97" t="s">
         <v>300</v>
@@ -4008,7 +4026,7 @@
         <v>1</v>
       </c>
       <c r="E97" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F97" t="s">
         <v>292</v>
@@ -4017,6 +4035,58 @@
         <v>1</v>
       </c>
       <c r="I97" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>301</v>
+      </c>
+      <c r="B98" t="s">
+        <v>278</v>
+      </c>
+      <c r="C98" t="s">
+        <v>300</v>
+      </c>
+      <c r="D98" t="s">
+        <v>1</v>
+      </c>
+      <c r="E98" t="s">
+        <v>303</v>
+      </c>
+      <c r="F98" t="s">
+        <v>292</v>
+      </c>
+      <c r="G98">
+        <v>2</v>
+      </c>
+      <c r="I98" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>302</v>
+      </c>
+      <c r="B99" t="s">
+        <v>295</v>
+      </c>
+      <c r="C99" t="s">
+        <v>300</v>
+      </c>
+      <c r="D99" t="s">
+        <v>1</v>
+      </c>
+      <c r="E99" t="s">
+        <v>305</v>
+      </c>
+      <c r="F99" t="s">
+        <v>292</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="I99" t="s">
         <v>307</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FIxes to side panel couplers
- Added PN122, a PTFE tube guide for between the pneumatic connectors for PN120
- Fixed outside panel coupler dimensions for new panel widths.
- Moved some brackets slightly to work with thicker floor panel.
- Modeled all remaining insulation and added relevant parts.
- Finished adding fasteners to the floor panels.
- Working on ensuring the air filtration both fits and can exhaust easily. This may require work, but is doable.
</commit_message>
<xml_diff>
--- a/BOM/Printed Part List.xlsx
+++ b/BOM/Printed Part List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jon\Documents\3D Print\Clockmaker\clock-3\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCE20833-40FD-43F5-B286-C56F64526A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87AC3BC8-1268-479D-A1D3-D5891885AD70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27255" yWindow="3405" windowWidth="23250" windowHeight="12480" xr2:uid="{7E6554FF-2F4B-4318-87E0-43D225F4F170}"/>
   </bookViews>
@@ -792,9 +792,6 @@
     <t>PTFE Coupling Guide</t>
   </si>
   <si>
-    <t>122 - Exterior - Frame - PTFE Coupling Guide.stl</t>
-  </si>
-  <si>
     <t>Bearing Alignment Slider</t>
   </si>
   <si>
@@ -1024,6 +1021,9 @@
   </si>
   <si>
     <t>088 - Electrical - Camera - Camera Stand.stl</t>
+  </si>
+  <si>
+    <t>122 - Exterior - Frame - PTFE Coupling Guide (TPU).stl</t>
   </si>
 </sst>
 </file>
@@ -1409,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC8DB31-6D45-4FED-94B6-5390BD4B0F2C}">
   <dimension ref="A1:I99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I94" sqref="I94"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H74" sqref="H74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1478,7 @@
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1504,7 +1504,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -1530,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -1556,7 +1556,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1582,7 +1582,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -1608,7 +1608,7 @@
         <v>1</v>
       </c>
       <c r="I7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1634,7 +1634,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -1660,7 +1660,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -1686,7 +1686,7 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -1712,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1738,7 +1738,7 @@
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1764,7 +1764,7 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1790,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="I14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1816,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1845,7 +1845,7 @@
         <v>94</v>
       </c>
       <c r="I16" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1871,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1897,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1926,7 +1926,7 @@
         <v>55</v>
       </c>
       <c r="I19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1952,7 +1952,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1978,7 +1978,7 @@
         <v>4</v>
       </c>
       <c r="I21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2004,7 +2004,7 @@
         <v>1</v>
       </c>
       <c r="I22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2030,7 +2030,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2056,7 +2056,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2082,7 +2082,7 @@
         <v>1</v>
       </c>
       <c r="I25" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2108,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="I26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2134,7 +2134,7 @@
         <v>1</v>
       </c>
       <c r="I27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2160,7 +2160,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
@@ -2186,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="I29" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2213,7 +2213,7 @@
       </c>
       <c r="H30" s="1"/>
       <c r="I30" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="H31" s="1"/>
       <c r="I31" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2267,7 +2267,7 @@
       </c>
       <c r="H32" s="1"/>
       <c r="I32" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2294,7 +2294,7 @@
       </c>
       <c r="H33" s="1"/>
       <c r="I33" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -2321,7 +2321,7 @@
       </c>
       <c r="H34" s="1"/>
       <c r="I34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
         <v>94</v>
       </c>
       <c r="I35" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2379,7 +2379,7 @@
         <v>94</v>
       </c>
       <c r="I36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2408,7 +2408,7 @@
         <v>94</v>
       </c>
       <c r="I37" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
         <v>94</v>
       </c>
       <c r="I38" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2466,7 +2466,7 @@
         <v>94</v>
       </c>
       <c r="I39" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2495,7 +2495,7 @@
         <v>94</v>
       </c>
       <c r="I40" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2524,7 +2524,7 @@
         <v>94</v>
       </c>
       <c r="I41" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2553,7 +2553,7 @@
         <v>94</v>
       </c>
       <c r="I42" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2582,7 +2582,7 @@
         <v>94</v>
       </c>
       <c r="I43" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2611,7 +2611,7 @@
         <v>176</v>
       </c>
       <c r="I44" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="H45" s="1"/>
       <c r="I45" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2667,7 +2667,7 @@
         <v>99</v>
       </c>
       <c r="I46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2696,7 +2696,7 @@
         <v>65</v>
       </c>
       <c r="I47" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2725,7 +2725,7 @@
         <v>65</v>
       </c>
       <c r="I48" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2751,7 +2751,7 @@
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
@@ -2777,7 +2777,7 @@
         <v>1</v>
       </c>
       <c r="I50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
         <v>94</v>
       </c>
       <c r="I51" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -2835,7 +2835,7 @@
         <v>94</v>
       </c>
       <c r="I52" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2861,7 +2861,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
@@ -2887,7 +2887,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2913,7 +2913,7 @@
         <v>1</v>
       </c>
       <c r="I55" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2939,7 +2939,7 @@
         <v>1</v>
       </c>
       <c r="I56" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -2968,7 +2968,7 @@
         <v>177</v>
       </c>
       <c r="I57" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2994,7 +2994,7 @@
         <v>1</v>
       </c>
       <c r="I58" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3020,7 +3020,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3046,7 +3046,7 @@
         <v>1</v>
       </c>
       <c r="I60" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3072,7 +3072,7 @@
         <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3101,7 +3101,7 @@
         <v>94</v>
       </c>
       <c r="I62" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3130,7 +3130,7 @@
         <v>240</v>
       </c>
       <c r="I63" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3156,7 +3156,7 @@
         <v>58</v>
       </c>
       <c r="I64" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
         <v>94</v>
       </c>
       <c r="I65" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3214,7 +3214,7 @@
         <v>94</v>
       </c>
       <c r="I66" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3240,7 +3240,7 @@
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3269,7 +3269,7 @@
         <v>94</v>
       </c>
       <c r="I68" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3286,7 +3286,7 @@
         <v>1</v>
       </c>
       <c r="E69" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F69" t="s">
         <v>35</v>
@@ -3295,7 +3295,7 @@
         <v>1</v>
       </c>
       <c r="I69" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3321,7 +3321,7 @@
         <v>16</v>
       </c>
       <c r="I70" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3347,7 +3347,7 @@
         <v>1</v>
       </c>
       <c r="I71" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3373,7 +3373,7 @@
         <v>2</v>
       </c>
       <c r="I72" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3749,12 +3749,12 @@
         <v>1</v>
       </c>
       <c r="I86" t="s">
-        <v>252</v>
+        <v>329</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B87" t="s">
         <v>36</v>
@@ -3766,7 +3766,7 @@
         <v>5</v>
       </c>
       <c r="E87" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F87" t="s">
         <v>35</v>
@@ -3775,12 +3775,12 @@
         <v>1</v>
       </c>
       <c r="I87" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B88" t="s">
         <v>36</v>
@@ -3792,7 +3792,7 @@
         <v>9</v>
       </c>
       <c r="E88" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F88" t="s">
         <v>35</v>
@@ -3801,7 +3801,7 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>